<commit_message>
mdl.medium_heat[t] == steam_heat_load[t] + mdl.DRHeatLoad[t] if t in peak else 削峰时段中品位热不能浪费
</commit_message>
<xml_diff>
--- a/DayAhead Electric DR.xlsx
+++ b/DayAhead Electric DR.xlsx
@@ -4865,13 +4865,13 @@
         <v>0.65550003</v>
       </c>
       <c r="G52">
-        <v>4290.11287176313</v>
+        <v>4290.11287176314</v>
       </c>
       <c r="H52">
         <v>4211.28022181818</v>
       </c>
       <c r="I52">
-        <v>212.719277345703</v>
+        <v>212.719277345702</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -4880,7 +4880,7 @@
         <v>10027.517996996</v>
       </c>
       <c r="L52">
-        <v>115.674884254297</v>
+        <v>115.674884254298</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -4960,13 +4960,13 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>412.315631254297</v>
+        <v>412.315631254298</v>
       </c>
       <c r="K53">
         <v>10029.9219870139</v>
       </c>
       <c r="L53">
-        <v>740.674884254297</v>
+        <v>740.674884254298</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -6167,7 +6167,7 @@
         <v>0</v>
       </c>
       <c r="K67">
-        <v>7195.39414412515</v>
+        <v>7195.39414412514</v>
       </c>
       <c r="L67">
         <v>0</v>
@@ -6597,7 +6597,7 @@
         <v>569.56987885</v>
       </c>
       <c r="K72">
-        <v>5962.37648358386</v>
+        <v>5962.37648358385</v>
       </c>
       <c r="L72">
         <v>625</v>
@@ -6849,7 +6849,7 @@
         <v>3143.43253181818</v>
       </c>
       <c r="I75">
-        <v>304.600822952324</v>
+        <v>304.600822952322</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -6861,7 +6861,7 @@
         <v>0</v>
       </c>
       <c r="M75">
-        <v>283.561518302324</v>
+        <v>283.561518302322</v>
       </c>
       <c r="N75">
         <v>1000</v>
@@ -13312,13 +13312,13 @@
         <v>0</v>
       </c>
       <c r="J53">
-        <v>8.243596646650991</v>
+        <v>8.243596646656901</v>
       </c>
       <c r="K53">
         <v>10002.4492020035</v>
       </c>
       <c r="L53">
-        <v>336.602849646651</v>
+        <v>336.602849646657</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -13398,13 +13398,13 @@
         <v>0</v>
       </c>
       <c r="J54">
-        <v>633.2785053466509</v>
+        <v>633.278505346657</v>
       </c>
       <c r="K54">
         <v>10057.3862557896</v>
       </c>
       <c r="L54">
-        <v>961.602849646651</v>
+        <v>961.602849646657</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -14175,7 +14175,7 @@
         <v>0</v>
       </c>
       <c r="K63">
-        <v>8404.0951933463</v>
+        <v>8404.095193346309</v>
       </c>
       <c r="L63">
         <v>0</v>
@@ -14433,7 +14433,7 @@
         <v>0</v>
       </c>
       <c r="K66">
-        <v>7356.84486894604</v>
+        <v>7356.84486894605</v>
       </c>
       <c r="L66">
         <v>0</v>
@@ -40002,13 +40002,13 @@
         <v>0</v>
       </c>
       <c r="J72">
-        <v>163.025129752051</v>
+        <v>163.02512975205</v>
       </c>
       <c r="K72">
         <v>5340.90232256832</v>
       </c>
       <c r="L72">
-        <v>218.455250902051</v>
+        <v>218.45525090205</v>
       </c>
       <c r="M72">
         <v>0</v>
@@ -40088,13 +40088,13 @@
         <v>0</v>
       </c>
       <c r="J73">
-        <v>799.832842072051</v>
+        <v>799.83284207205</v>
       </c>
       <c r="K73">
         <v>5379.43318885113</v>
       </c>
       <c r="L73">
-        <v>843.455250902051</v>
+        <v>843.45525090205</v>
       </c>
       <c r="M73">
         <v>0</v>

</xml_diff>